<commit_message>
update methods to connect to snowpark
</commit_message>
<xml_diff>
--- a/SQL/SNOWFLAKE_SQL_EXAMPLES.xlsx
+++ b/SQL/SNOWFLAKE_SQL_EXAMPLES.xlsx
@@ -18,7 +18,7 @@
   </sheets>
   <calcPr calcId="162913"/>
   <pivotCaches>
-    <pivotCache cacheId="3" r:id="rId4"/>
+    <pivotCache cacheId="0" r:id="rId4"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -4632,7 +4632,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
-    <numFmt numFmtId="170" formatCode="dd\/mm\/yyyy\ hh:mm:ss"/>
+    <numFmt numFmtId="164" formatCode="dd\/mm\/yyyy\ hh:mm:ss"/>
   </numFmts>
   <fonts count="5">
     <font>
@@ -4747,8 +4747,8 @@
     </xf>
     <xf numFmtId="47" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -5499,7 +5499,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="3" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="G11:H15" firstHeaderRow="1" firstDataRow="1" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
   <pivotFields count="5">
     <pivotField showAll="0"/>
@@ -5837,8 +5837,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H94"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="B39" sqref="B39"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5847,7 +5847,7 @@
     <col min="2" max="2" width="37" customWidth="1"/>
     <col min="3" max="3" width="21.7109375" customWidth="1"/>
     <col min="4" max="4" width="15" customWidth="1"/>
-    <col min="5" max="5" width="34.7109375" customWidth="1"/>
+    <col min="5" max="5" width="34.7109375" hidden="1" customWidth="1"/>
     <col min="6" max="6" width="13" customWidth="1"/>
     <col min="7" max="7" width="13.140625" customWidth="1"/>
     <col min="8" max="8" width="13.5703125" customWidth="1"/>

</xml_diff>